<commit_message>
group figure as DHFR fragment position
</commit_message>
<xml_diff>
--- a/label.xlsx
+++ b/label.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000weng_lab\data_R\growth_curve\20250420\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4895770C-91BF-4479-A47A-8FA094F6C745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C22C54-9A4C-4CD6-9A23-7D3A0BB4641F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="250">
   <si>
     <t>plasmid</t>
   </si>
@@ -415,7 +415,6 @@
   </si>
   <si>
     <t>RNA7SK</t>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>plasmid</t>
@@ -767,26 +766,27 @@
   </si>
   <si>
     <t>I15</t>
+  </si>
+  <si>
+    <t>DHFR3_C_term</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DHFR12_N_term</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -816,11 +816,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1127,35 +1124,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1644,7 +1641,7 @@
         <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
         <v>13</v>
@@ -1670,7 +1667,7 @@
         <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -1696,7 +1693,7 @@
         <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="G22" t="s">
         <v>13</v>
@@ -3038,6 +3035,12 @@
       <c r="B74" t="s">
         <v>117</v>
       </c>
+      <c r="E74" t="s">
+        <v>248</v>
+      </c>
+      <c r="F74" t="s">
+        <v>249</v>
+      </c>
       <c r="G74" t="s">
         <v>118</v>
       </c>
@@ -3052,6 +3055,12 @@
       <c r="B75" t="s">
         <v>119</v>
       </c>
+      <c r="E75" t="s">
+        <v>248</v>
+      </c>
+      <c r="F75" t="s">
+        <v>249</v>
+      </c>
       <c r="G75" t="s">
         <v>118</v>
       </c>
@@ -3066,6 +3075,12 @@
       <c r="B76" t="s">
         <v>120</v>
       </c>
+      <c r="E76" t="s">
+        <v>38</v>
+      </c>
+      <c r="F76" t="s">
+        <v>12</v>
+      </c>
       <c r="G76" t="s">
         <v>118</v>
       </c>
@@ -3080,6 +3095,12 @@
       <c r="B77" t="s">
         <v>122</v>
       </c>
+      <c r="E77" t="s">
+        <v>38</v>
+      </c>
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
       <c r="G77" t="s">
         <v>129</v>
       </c>
@@ -3094,6 +3115,12 @@
       <c r="B78" t="s">
         <v>123</v>
       </c>
+      <c r="E78" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
       <c r="G78" t="s">
         <v>129</v>
       </c>
@@ -3108,6 +3135,12 @@
       <c r="B79" t="s">
         <v>124</v>
       </c>
+      <c r="E79" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" t="s">
+        <v>12</v>
+      </c>
       <c r="G79" t="s">
         <v>129</v>
       </c>
@@ -3122,6 +3155,12 @@
       <c r="B80" t="s">
         <v>126</v>
       </c>
+      <c r="E80" t="s">
+        <v>38</v>
+      </c>
+      <c r="F80" t="s">
+        <v>12</v>
+      </c>
       <c r="G80" t="s">
         <v>118</v>
       </c>
@@ -3136,6 +3175,12 @@
       <c r="B81" t="s">
         <v>127</v>
       </c>
+      <c r="E81" t="s">
+        <v>38</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
       <c r="G81" t="s">
         <v>118</v>
       </c>
@@ -3150,6 +3195,12 @@
       <c r="B82" t="s">
         <v>128</v>
       </c>
+      <c r="E82" t="s">
+        <v>38</v>
+      </c>
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
       <c r="G82" t="s">
         <v>118</v>
       </c>
@@ -3158,7 +3209,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -3168,7 +3219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D18" sqref="A1:H73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -3683,7 +3736,7 @@
         <v>170</v>
       </c>
       <c r="F20" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="G20" t="s">
         <v>145</v>
@@ -3709,7 +3762,7 @@
         <v>170</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="G21" t="s">
         <v>145</v>
@@ -3735,7 +3788,7 @@
         <v>170</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="G22" t="s">
         <v>145</v>
@@ -5071,7 +5124,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>